<commit_message>
hello message and logging
</commit_message>
<xml_diff>
--- a/qa.xlsx
+++ b/qa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhozh/Desktop/projects/python/bots/pelican_helper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6529E33C-EC23-8C4E-88AC-2D0FE4ADE231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272FF5A8-4132-154D-989B-BA700CFE1473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -619,9 +619,6 @@
     <t>При условии свободного бюджетного места и твоей хорошей успеваемости можно попробовать перевестить с контрактной на бюджетную форму обучения, обратись с этим вопросом в дирекцию своего института</t>
   </si>
   <si>
-    <t>перевод на бюджет</t>
-  </si>
-  <si>
     <t>Можно ли создать своё объединение?</t>
   </si>
   <si>
@@ -879,9 +876,6 @@
   </si>
   <si>
     <t>Каждый год это разные секции. Вся информация транслируется здесь https://vk.com/sport.spbstu.</t>
-  </si>
-  <si>
-    <t>секции нет разрядов</t>
   </si>
   <si>
     <t>Если меня записали в спец.группу, то я занимаюсь где-то в другом месте от своих одногруппников?</t>
@@ -1935,9 +1929,6 @@
   </si>
   <si>
     <t>Мне трудно сказать, где будет учиться именно твоя группа, всё-таки Политех не такой уж маленький. Однако есть карта кампуса, благодаря которой ты быстро найдёшь для себя ответ (https://www.spbstu.ru/campus-map/index.php).</t>
-  </si>
-  <si>
-    <t>корпус учиться</t>
   </si>
   <si>
     <t>Где можно посмотреть расписание?</t>
@@ -2940,9 +2931,6 @@
     <t>прогул пар</t>
   </si>
   <si>
-    <t>добраться до универ путь ехать</t>
-  </si>
-  <si>
     <t>проблем здоровье</t>
   </si>
   <si>
@@ -3397,6 +3385,18 @@
   </si>
   <si>
     <t>сборная спорт</t>
+  </si>
+  <si>
+    <t>перевод бюджет</t>
+  </si>
+  <si>
+    <t>секции разрядов</t>
+  </si>
+  <si>
+    <t>добраться универ путь ехать</t>
+  </si>
+  <si>
+    <t>корпус учиться кампус</t>
   </si>
 </sst>
 </file>
@@ -4247,8 +4247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C249" zoomScale="119" workbookViewId="0">
-      <selection activeCell="C251" sqref="C251"/>
+    <sheetView tabSelected="1" topLeftCell="C251" zoomScale="119" workbookViewId="0">
+      <selection activeCell="C254" sqref="C254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4283,7 +4283,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="32">
@@ -4291,7 +4291,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32">
@@ -4302,7 +4302,7 @@
         <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="112">
@@ -4313,7 +4313,7 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="71">
@@ -4324,7 +4324,7 @@
         <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="176">
@@ -4335,7 +4335,7 @@
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="96">
@@ -4346,7 +4346,7 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="32">
@@ -4357,7 +4357,7 @@
         <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="64">
@@ -4368,7 +4368,7 @@
         <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4382,7 +4382,7 @@
         <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="64">
@@ -4393,7 +4393,7 @@
         <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4421,7 +4421,7 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="32">
@@ -4432,7 +4432,7 @@
         <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="48">
@@ -4443,7 +4443,7 @@
         <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="48">
@@ -4454,7 +4454,7 @@
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="32">
@@ -4465,7 +4465,7 @@
         <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="112">
@@ -4476,7 +4476,7 @@
         <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="32">
@@ -4487,7 +4487,7 @@
         <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="48">
@@ -4498,7 +4498,7 @@
         <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="48">
@@ -4509,7 +4509,7 @@
         <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="48">
@@ -4520,7 +4520,7 @@
         <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="48">
@@ -4531,7 +4531,7 @@
         <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16">
@@ -4542,7 +4542,7 @@
         <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="288">
@@ -4553,7 +4553,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="32">
@@ -4564,7 +4564,7 @@
         <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="48">
@@ -4575,7 +4575,7 @@
         <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16">
@@ -4586,7 +4586,7 @@
         <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="32">
@@ -4597,7 +4597,7 @@
         <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="64">
@@ -4608,7 +4608,7 @@
         <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="64">
@@ -4630,7 +4630,7 @@
         <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="61">
@@ -4641,7 +4641,7 @@
         <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="32">
@@ -4674,7 +4674,7 @@
         <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="128">
@@ -4685,7 +4685,7 @@
         <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="64">
@@ -4696,62 +4696,62 @@
         <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="80">
       <c r="A45" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="80">
       <c r="A46" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="192">
       <c r="A47" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="48">
       <c r="A48" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="16">
       <c r="A49" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C49" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="48">
@@ -4762,7 +4762,7 @@
         <v>88</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="32">
@@ -4784,7 +4784,7 @@
         <v>93</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="64">
@@ -4795,7 +4795,7 @@
         <v>95</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="64">
@@ -4806,7 +4806,7 @@
         <v>97</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="64">
@@ -4817,7 +4817,7 @@
         <v>99</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="96">
@@ -4828,7 +4828,7 @@
         <v>101</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="64">
@@ -4839,7 +4839,7 @@
         <v>103</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="48">
@@ -4850,7 +4850,7 @@
         <v>105</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="80">
@@ -4861,7 +4861,7 @@
         <v>107</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="80">
@@ -4872,7 +4872,7 @@
         <v>109</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="112">
@@ -4883,7 +4883,7 @@
         <v>111</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="48">
@@ -4894,7 +4894,7 @@
         <v>113</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="96">
@@ -4916,7 +4916,7 @@
         <v>118</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="48">
@@ -4927,7 +4927,7 @@
         <v>120</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="32">
@@ -4938,7 +4938,7 @@
         <v>122</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="64">
@@ -4949,7 +4949,7 @@
         <v>124</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="48">
@@ -4960,7 +4960,7 @@
         <v>126</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="32">
@@ -4982,7 +4982,7 @@
         <v>131</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="48">
@@ -4993,7 +4993,7 @@
         <v>133</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="48">
@@ -5004,7 +5004,7 @@
         <v>135</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="64">
@@ -5015,7 +5015,7 @@
         <v>137</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="32">
@@ -5026,7 +5026,7 @@
         <v>139</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="48">
@@ -5037,7 +5037,7 @@
         <v>141</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="64">
@@ -5048,7 +5048,7 @@
         <v>143</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="16">
@@ -5059,7 +5059,7 @@
         <v>145</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="48">
@@ -5070,161 +5070,161 @@
         <v>147</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>148</v>
+        <v>888</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="48">
       <c r="A79" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B79" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="C79" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="38">
       <c r="A80" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="18">
       <c r="A81" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="C81" s="2" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="32">
       <c r="A82" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="C82" s="2" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="105">
       <c r="A83" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B83" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="26" t="s">
-        <v>165</v>
-      </c>
       <c r="C83" s="2" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="38">
       <c r="A84" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="B84" s="28" t="s">
-        <v>167</v>
-      </c>
       <c r="C84" s="2" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="60">
       <c r="A85" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="29" t="s">
-        <v>169</v>
-      </c>
       <c r="C85" s="2" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="71">
       <c r="A86" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="30" t="s">
-        <v>171</v>
-      </c>
       <c r="C86" s="2" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="85">
       <c r="A87" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="30" t="s">
-        <v>173</v>
-      </c>
       <c r="C87" s="2" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="113">
       <c r="A88" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="30" t="s">
-        <v>175</v>
-      </c>
       <c r="C88" s="2" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="64">
       <c r="A89" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="C89" s="2" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="32">
       <c r="A90" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="C90" s="2" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="38">
       <c r="A91" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="C91" s="2" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="38">
       <c r="A92" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="C92" s="2" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="18">
@@ -5233,134 +5233,134 @@
     </row>
     <row r="94" spans="1:3" ht="32">
       <c r="A94" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="C94" s="2" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="32">
       <c r="A95" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="C95" s="2" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="48">
       <c r="A96" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="C96" s="2" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="48">
       <c r="A97" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="76">
       <c r="A98" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="C98" s="2" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="48">
       <c r="A99" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="C99" s="2" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="32">
       <c r="A100" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="C100" s="2" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="136">
       <c r="A101" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="B101" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="B101" s="32" t="s">
-        <v>200</v>
-      </c>
       <c r="C101" s="2" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="38">
       <c r="A102" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="C102" s="2" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="18">
       <c r="A103" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="C103" s="2" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="32">
       <c r="A104" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="C104" s="2" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="120">
       <c r="A105" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="B105" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="B105" s="26" t="s">
-        <v>208</v>
-      </c>
       <c r="C105" s="2" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="18">
@@ -5374,150 +5374,150 @@
     </row>
     <row r="108" spans="1:3" ht="48">
       <c r="A108" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="C108" s="2" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="57">
       <c r="A109" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="95">
       <c r="A110" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B110" s="30" t="s">
-        <v>213</v>
-      </c>
       <c r="C110" s="2" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="57">
       <c r="A111" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="C111" s="2" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="57">
       <c r="A112" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="61">
       <c r="A113" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="B113" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="B113" s="34" t="s">
-        <v>218</v>
-      </c>
       <c r="C113" s="2" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="57">
       <c r="A114" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="C114" s="2" t="s">
-        <v>221</v>
+        <v>889</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="57">
       <c r="A115" s="24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="57">
       <c r="A116" s="24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="153">
       <c r="A117" s="24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B117" s="35" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="38">
       <c r="A118" s="24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="57">
       <c r="A119" s="24" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="38">
       <c r="A120" s="24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="57">
       <c r="A121" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="18">
@@ -5530,35 +5530,35 @@
     </row>
     <row r="124" spans="1:3" ht="48">
       <c r="A124" s="24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="38">
       <c r="A125" s="24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="38">
       <c r="A126" s="24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="18">
@@ -5567,156 +5567,156 @@
     </row>
     <row r="128" spans="1:3" ht="32">
       <c r="A128" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="18">
       <c r="A129" s="25" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="32">
       <c r="A130" s="25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="19">
       <c r="A131" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="32">
       <c r="A132" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="48">
       <c r="A133" s="25" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="34">
       <c r="A134" s="25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B134" s="36" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="18">
       <c r="A135" s="25" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="18">
       <c r="A136" s="37" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="224">
       <c r="A137" s="38" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B137" s="17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="39" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B138" s="38"/>
       <c r="C138" s="38" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="48">
       <c r="A139" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B139" s="14" t="s">
         <v>128</v>
       </c>
       <c r="C139" s="38" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="64">
       <c r="A140" s="39" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B140" s="14" t="s">
         <v>95</v>
       </c>
       <c r="C140" s="17" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="80">
       <c r="A141" s="39" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C141" s="17" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="48">
       <c r="A142" s="40" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B142" s="38"/>
       <c r="C142" s="38"/>
@@ -5728,134 +5728,134 @@
     </row>
     <row r="144" spans="1:3" ht="32">
       <c r="A144" s="39" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C144" s="38" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="192">
       <c r="A145" s="39" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B145" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C145" s="38" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="64">
       <c r="A146" s="39" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B146" s="14" t="s">
         <v>103</v>
       </c>
       <c r="C146" s="38" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="41" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B147" s="38"/>
       <c r="C147" s="38"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="39" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B148" s="38" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C148" s="38" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="39" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B149" s="38" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C149" s="38" t="s">
-        <v>739</v>
+        <v>890</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B150" s="38"/>
       <c r="C150" s="38" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="B151" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="C151" s="38" t="s">
         <v>280</v>
-      </c>
-      <c r="B151" s="38" t="s">
-        <v>281</v>
-      </c>
-      <c r="C151" s="38" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="41" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B152" s="38"/>
       <c r="C152" s="38" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="32">
       <c r="A153" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B153" s="38" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C153" s="38" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="192">
       <c r="A154" s="39" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B154" s="17" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C154" s="38" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="64">
       <c r="A155" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B155" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C155" s="38" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="39" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B156" s="38" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C156" s="38" t="s">
         <v>116</v>
@@ -5863,24 +5863,24 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="39" t="s">
+        <v>290</v>
+      </c>
+      <c r="B157" s="38" t="s">
+        <v>291</v>
+      </c>
+      <c r="C157" s="38" t="s">
         <v>292</v>
-      </c>
-      <c r="B157" s="38" t="s">
-        <v>293</v>
-      </c>
-      <c r="C157" s="38" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="32">
       <c r="A158" s="39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B158" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C158" s="38" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -5890,167 +5890,167 @@
     </row>
     <row r="160" spans="1:3" ht="32">
       <c r="A160" s="39" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C160" s="38" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="B161" s="38" t="s">
+        <v>298</v>
+      </c>
+      <c r="C161" s="38" t="s">
         <v>299</v>
-      </c>
-      <c r="B161" s="38" t="s">
-        <v>300</v>
-      </c>
-      <c r="C161" s="38" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="39" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B162" s="38" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C162" s="38" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="48">
       <c r="A163" s="39" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B163" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C163" s="38" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="39" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B164" s="38" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C164" s="38" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B165" s="38" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C165" s="38" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="39" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B166" s="38" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C166" s="38" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="39" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B167" s="38" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C167" s="38" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="B168" s="38" t="s">
+        <v>312</v>
+      </c>
+      <c r="C168" s="38" t="s">
         <v>313</v>
-      </c>
-      <c r="B168" s="38" t="s">
-        <v>314</v>
-      </c>
-      <c r="C168" s="38" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="32">
       <c r="A169" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="B169" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="C169" s="38" t="s">
         <v>316</v>
-      </c>
-      <c r="B169" s="38" t="s">
-        <v>317</v>
-      </c>
-      <c r="C169" s="38" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="B170" s="38" t="s">
+        <v>318</v>
+      </c>
+      <c r="C170" s="38" t="s">
         <v>319</v>
-      </c>
-      <c r="B170" s="38" t="s">
-        <v>320</v>
-      </c>
-      <c r="C170" s="38" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="39" t="s">
+        <v>320</v>
+      </c>
+      <c r="B171" s="38" t="s">
+        <v>321</v>
+      </c>
+      <c r="C171" s="38" t="s">
         <v>322</v>
-      </c>
-      <c r="B171" s="38" t="s">
-        <v>323</v>
-      </c>
-      <c r="C171" s="38" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="B172" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="C172" s="38" t="s">
         <v>325</v>
-      </c>
-      <c r="B172" s="38" t="s">
-        <v>326</v>
-      </c>
-      <c r="C172" s="38" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="16">
       <c r="A173" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="B173" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="C173" s="38" t="s">
         <v>328</v>
-      </c>
-      <c r="B173" s="38" t="s">
-        <v>329</v>
-      </c>
-      <c r="C173" s="38" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="32">
       <c r="A174" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B174" s="38" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C174" s="38" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -6060,46 +6060,46 @@
     </row>
     <row r="176" spans="1:3" ht="80">
       <c r="A176" s="39" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B176" s="14" t="s">
         <v>75</v>
       </c>
       <c r="C176" s="38" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="39" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B177" s="38" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C177" s="38" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="64">
       <c r="A178" s="39" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B178" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C178" s="38" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="48">
       <c r="A179" s="39" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B179" s="14" t="s">
         <v>88</v>
       </c>
       <c r="C179" s="38" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -6109,24 +6109,24 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="39" t="s">
+        <v>337</v>
+      </c>
+      <c r="B181" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="C181" s="38" t="s">
         <v>339</v>
-      </c>
-      <c r="B181" s="38" t="s">
-        <v>340</v>
-      </c>
-      <c r="C181" s="38" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="42" t="s">
+        <v>340</v>
+      </c>
+      <c r="B182" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="C182" s="38" t="s">
         <v>342</v>
-      </c>
-      <c r="B182" s="38" t="s">
-        <v>343</v>
-      </c>
-      <c r="C182" s="38" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -6136,20 +6136,20 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="41" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B184" s="38"/>
       <c r="C184" s="38"/>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="B185" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="C185" s="38" t="s">
         <v>346</v>
-      </c>
-      <c r="B185" s="38" t="s">
-        <v>347</v>
-      </c>
-      <c r="C185" s="38" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -6159,192 +6159,192 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="39" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B187" s="38" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C187" s="38" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="39" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B188" s="38" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C188" s="38" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="48">
       <c r="A189" s="39" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B189" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C189" s="38" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="32">
       <c r="A190" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="B190" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="C190" s="38" t="s">
         <v>355</v>
-      </c>
-      <c r="B190" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="C190" s="38" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="39" t="s">
+        <v>356</v>
+      </c>
+      <c r="B191" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="C191" s="38" t="s">
         <v>358</v>
-      </c>
-      <c r="B191" s="38" t="s">
-        <v>359</v>
-      </c>
-      <c r="C191" s="38" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="48">
       <c r="A192" s="39" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B192" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C192" s="38" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="48">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="64">
       <c r="A193" s="39" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C193" s="38" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="48">
       <c r="A194" s="39" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C194" s="38" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="16">
       <c r="A195" s="39" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C195" s="38" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="41" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B196" s="38"/>
       <c r="C196" s="38"/>
     </row>
     <row r="197" spans="1:3" ht="64">
       <c r="A197" s="40" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B197" s="38"/>
       <c r="C197" s="38"/>
     </row>
     <row r="198" spans="1:3" ht="29">
       <c r="A198" s="43" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B198" s="44" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C198" s="60" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="57">
       <c r="A199" s="43" t="s">
+        <v>370</v>
+      </c>
+      <c r="B199" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="C199" s="45" t="s">
         <v>372</v>
-      </c>
-      <c r="B199" s="46" t="s">
-        <v>373</v>
-      </c>
-      <c r="C199" s="45" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="29">
       <c r="A200" s="43" t="s">
+        <v>373</v>
+      </c>
+      <c r="B200" s="47" t="s">
+        <v>374</v>
+      </c>
+      <c r="C200" s="45" t="s">
         <v>375</v>
-      </c>
-      <c r="B200" s="47" t="s">
-        <v>376</v>
-      </c>
-      <c r="C200" s="45" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="43">
       <c r="A201" s="43" t="s">
+        <v>376</v>
+      </c>
+      <c r="B201" s="46" t="s">
+        <v>377</v>
+      </c>
+      <c r="C201" s="45" t="s">
         <v>378</v>
-      </c>
-      <c r="B201" s="46" t="s">
-        <v>379</v>
-      </c>
-      <c r="C201" s="45" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="43">
       <c r="A202" s="43" t="s">
+        <v>379</v>
+      </c>
+      <c r="B202" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="C202" s="45" t="s">
         <v>381</v>
-      </c>
-      <c r="B202" s="46" t="s">
-        <v>382</v>
-      </c>
-      <c r="C202" s="45" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="57">
       <c r="A203" s="43" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B203" s="46" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C203" s="60" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="169">
       <c r="A204" s="43" t="s">
+        <v>384</v>
+      </c>
+      <c r="B204" s="46" t="s">
+        <v>385</v>
+      </c>
+      <c r="C204" s="45" t="s">
         <v>386</v>
-      </c>
-      <c r="B204" s="46" t="s">
-        <v>387</v>
-      </c>
-      <c r="C204" s="45" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="16">
@@ -6352,1404 +6352,1404 @@
     </row>
     <row r="206" spans="1:3" ht="43">
       <c r="A206" s="43" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B206" s="48" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C206" s="60" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="71">
       <c r="A207" s="43" t="s">
+        <v>389</v>
+      </c>
+      <c r="B207" s="46" t="s">
+        <v>390</v>
+      </c>
+      <c r="C207" s="45" t="s">
         <v>391</v>
       </c>
-      <c r="B207" s="46" t="s">
+    </row>
+    <row r="208" spans="1:3" ht="71">
+      <c r="A208" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="C207" s="45" t="s">
+      <c r="B208" s="46" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" ht="57">
-      <c r="A208" s="43" t="s">
-        <v>394</v>
-      </c>
-      <c r="B208" s="46" t="s">
-        <v>395</v>
-      </c>
       <c r="C208" s="60" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="43">
       <c r="A209" s="43" t="s">
+        <v>394</v>
+      </c>
+      <c r="B209" s="49" t="s">
+        <v>395</v>
+      </c>
+      <c r="C209" s="45" t="s">
         <v>396</v>
-      </c>
-      <c r="B209" s="49" t="s">
-        <v>397</v>
-      </c>
-      <c r="C209" s="45" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="29">
       <c r="A210" s="43" t="s">
+        <v>397</v>
+      </c>
+      <c r="B210" s="46" t="s">
+        <v>398</v>
+      </c>
+      <c r="C210" s="45" t="s">
         <v>399</v>
-      </c>
-      <c r="B210" s="46" t="s">
-        <v>400</v>
-      </c>
-      <c r="C210" s="45" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="43">
       <c r="A211" s="43" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B211" s="46" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C211" s="60" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="17">
       <c r="A212" s="43" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B212" s="46" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="85">
       <c r="A213" s="43" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B213" s="48" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C213" s="60" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="136">
       <c r="A214" s="43" t="s">
+        <v>406</v>
+      </c>
+      <c r="B214" s="50" t="s">
+        <v>407</v>
+      </c>
+      <c r="C214" s="45" t="s">
         <v>408</v>
-      </c>
-      <c r="B214" s="50" t="s">
-        <v>409</v>
-      </c>
-      <c r="C214" s="45" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="34">
       <c r="A215" s="43" t="s">
+        <v>409</v>
+      </c>
+      <c r="B215" s="49" t="s">
+        <v>410</v>
+      </c>
+      <c r="C215" s="45" t="s">
         <v>411</v>
-      </c>
-      <c r="B215" s="49" t="s">
-        <v>412</v>
-      </c>
-      <c r="C215" s="45" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="17">
       <c r="A216" s="43" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B216" s="46" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="43">
       <c r="A217" s="51" t="s">
+        <v>413</v>
+      </c>
+      <c r="B217" s="49" t="s">
+        <v>414</v>
+      </c>
+      <c r="C217" s="45" t="s">
         <v>415</v>
-      </c>
-      <c r="B217" s="49" t="s">
-        <v>416</v>
-      </c>
-      <c r="C217" s="45" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="202">
       <c r="A218" s="52" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B218" s="49" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C218" s="60" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="43">
       <c r="A219" s="43" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B219" s="49" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C219" s="60" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="43">
       <c r="A220" s="43" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B220" s="48" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C220" s="60" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="60">
       <c r="A221" s="43" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B221" s="49" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C221" s="60" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="43">
       <c r="A222" s="43" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B222" s="48" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C222" s="60" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="43">
       <c r="A223" s="43" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B223" s="49" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C223" s="60" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="29">
       <c r="A224" s="43" t="s">
+        <v>428</v>
+      </c>
+      <c r="B224" s="49" t="s">
+        <v>429</v>
+      </c>
+      <c r="C224" s="45" t="s">
         <v>430</v>
-      </c>
-      <c r="B224" s="49" t="s">
-        <v>431</v>
-      </c>
-      <c r="C224" s="45" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="34">
       <c r="A225" s="43" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B225" s="46" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="43">
       <c r="A226" s="43" t="s">
+        <v>432</v>
+      </c>
+      <c r="B226" s="48" t="s">
+        <v>433</v>
+      </c>
+      <c r="C226" s="45" t="s">
         <v>434</v>
-      </c>
-      <c r="B226" s="48" t="s">
-        <v>435</v>
-      </c>
-      <c r="C226" s="45" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="57">
       <c r="A227" s="53" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B227" s="54" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C227" s="61" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="57">
       <c r="A228" s="53" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B228" s="53" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C228" s="61" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="57">
       <c r="A229" s="53" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B229" s="53" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C229" s="61" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="133">
       <c r="A230" s="53" t="s">
+        <v>441</v>
+      </c>
+      <c r="B230" s="53" t="s">
+        <v>442</v>
+      </c>
+      <c r="C230" s="53" t="s">
         <v>443</v>
-      </c>
-      <c r="B230" s="53" t="s">
-        <v>444</v>
-      </c>
-      <c r="C230" s="53" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="152">
       <c r="A231" s="53" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B231" s="53" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C231" s="61" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="190">
       <c r="A232" s="53" t="s">
+        <v>445</v>
+      </c>
+      <c r="B232" s="53" t="s">
+        <v>446</v>
+      </c>
+      <c r="C232" s="53" t="s">
         <v>447</v>
-      </c>
-      <c r="B232" s="53" t="s">
-        <v>448</v>
-      </c>
-      <c r="C232" s="53" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="95">
       <c r="A233" s="53" t="s">
+        <v>448</v>
+      </c>
+      <c r="B233" s="53" t="s">
+        <v>449</v>
+      </c>
+      <c r="C233" s="53" t="s">
         <v>450</v>
-      </c>
-      <c r="B233" s="53" t="s">
-        <v>451</v>
-      </c>
-      <c r="C233" s="53" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="171">
       <c r="A234" s="53" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B234" s="53" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C234" s="61" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="114">
       <c r="A235" s="53" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B235" s="53" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C235" s="53" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="190">
       <c r="A236" s="53" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B236" s="53" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C236" s="61" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="76">
       <c r="A237" s="53" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B237" s="55" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C237" s="61" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="114">
       <c r="A238" s="53" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B238" s="53" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C238" s="61" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="133">
       <c r="A239" s="53" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B239" s="53" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C239" s="61" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="190">
       <c r="A240" s="53" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B240" s="53" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C240" s="61" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="114">
       <c r="A241" s="53" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B241" s="53" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C241" s="61" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="95">
       <c r="A242" s="53" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B242" s="53" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C242" s="61" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="57">
       <c r="A243" s="53" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B243" s="55" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C243" s="61" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="76">
       <c r="A244" s="53" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B244" s="53" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C244" s="61" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="245" spans="1:3" ht="38">
       <c r="A245" s="53" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B245" s="53" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C245" s="61" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="76">
       <c r="A246" s="53" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B246" s="55" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C246" s="61" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="57">
       <c r="A247" s="53" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B247" s="53" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C247" s="61" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="228">
       <c r="A248" s="53" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B248" s="53" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C248" s="53" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="249" spans="1:3" ht="114">
       <c r="A249" s="53" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B249" s="53" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C249" s="53" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="250" spans="1:3" ht="114">
       <c r="A250" s="53" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B250" s="53" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C250" s="53" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="95">
       <c r="A251" s="53" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B251" s="53" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C251" s="53" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
     </row>
     <row r="252" spans="1:3" ht="38">
       <c r="A252" s="53" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B252" s="53" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C252" s="53" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="133">
       <c r="A253" s="53" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B253" s="53" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C253" s="53" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="95">
       <c r="A254" s="53" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B254" s="53" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C254" s="53" t="s">
-        <v>493</v>
+        <v>891</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="38">
       <c r="A255" s="53" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B255" s="53" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C255" s="53" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="256" spans="1:3" ht="171">
       <c r="A256" s="53" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B256" s="53" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C256" s="61" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="257" spans="1:3" ht="114">
       <c r="A257" s="53" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B257" s="53" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C257" s="53" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="209">
       <c r="A258" s="53" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B258" s="53" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C258" s="53" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="114">
       <c r="A259" s="53" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B259" s="53" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C259" s="53" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="114">
       <c r="A260" s="53" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B260" s="53" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C260" s="53" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="261" spans="1:3" ht="190">
       <c r="A261" s="53" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B261" s="53" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C261" s="53" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="114">
       <c r="A262" s="53" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B262" s="53" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C262" s="53" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="228">
       <c r="A263" s="53" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B263" s="53" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C263" s="53" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
     </row>
     <row r="264" spans="1:3" ht="95">
       <c r="A264" s="53" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B264" s="53" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C264" s="61" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="114">
       <c r="A265" s="53" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B265" s="53" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C265" s="53" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="266" spans="1:3" ht="76">
       <c r="A266" s="53" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B266" s="53" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C266" s="53" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="114">
       <c r="A267" s="53" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B267" s="53" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C267" s="53" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
     </row>
     <row r="268" spans="1:3" ht="57">
       <c r="A268" s="53" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B268" s="53" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C268" s="61" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="95">
       <c r="A269" s="53" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B269" s="53" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C269" s="53" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="76">
       <c r="A270" s="53" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B270" s="53" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C270" s="53" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="271" spans="1:3" ht="95">
       <c r="A271" s="53" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B271" s="53" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C271" s="53" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="95">
       <c r="A272" s="53" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B272" s="53" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C272" s="53" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="152">
       <c r="A273" s="53" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B273" s="53" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C273" s="61" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="274" spans="1:3" ht="114">
       <c r="A274" s="53" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B274" s="53" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C274" s="53" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="275" spans="1:3" ht="76">
       <c r="A275" s="53" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B275" s="55" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C275" s="53" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="57">
       <c r="A276" s="53" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B276" s="56" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C276" s="53" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="57">
       <c r="A277" s="53" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B277" s="57" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C277" s="61" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="57">
       <c r="A278" s="53" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B278" s="53" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C278" s="53" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="114">
       <c r="A279" s="53" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B279" s="55" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C279" s="53" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="112">
       <c r="A280" s="18" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B280" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C280" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="192">
       <c r="A281" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B281" s="13" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C281" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="282" spans="1:3" ht="409.6">
       <c r="A282" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B282" s="19" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C282" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="96">
       <c r="A283" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C283" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="80">
       <c r="A284" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C284" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="285" spans="1:3" ht="80">
       <c r="A285" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B285" s="13" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C285" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="286" spans="1:3" ht="96">
       <c r="A286" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B286" s="13" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C286" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
     <row r="287" spans="1:3" ht="144">
       <c r="A287" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B287" s="13" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C287" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="288" spans="1:3" ht="80">
       <c r="A288" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B288" s="13" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C288" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
     </row>
     <row r="289" spans="1:3" ht="32">
       <c r="A289" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B289" s="13" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C289" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="290" spans="1:3" ht="96">
       <c r="A290" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B290" s="13" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C290" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="176">
       <c r="A291" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B291" s="13" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C291" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="365">
       <c r="A292" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B292" s="13" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C292" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="293" spans="1:3" ht="112">
       <c r="A293" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B293" s="13" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C293" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="409.6">
       <c r="A294" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B294" s="13" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C294" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="224">
       <c r="A295" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B295" s="58" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C295" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
     </row>
     <row r="296" spans="1:3" ht="288">
       <c r="A296" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B296" s="13" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C296" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="96">
       <c r="A297" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B297" s="13" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C297" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="16">
       <c r="A298" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B298" s="13" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C298" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="32">
       <c r="A299" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B299" s="13" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C299" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="32">
       <c r="A300" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B300" s="13" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C300" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="301" spans="1:3" ht="80">
       <c r="A301" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B301" s="13" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C301" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B302" s="13"/>
     </row>
     <row r="303" spans="1:3" ht="48">
       <c r="A303" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B303" s="13" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C303" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="304" spans="1:3" ht="208">
       <c r="A304" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B304" s="13" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C304" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="80">
       <c r="A305" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B305" s="13" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C305" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="48">
       <c r="A306" s="2" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B306" s="13" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C306" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="176">
       <c r="A307" s="2" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C307" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="192">
       <c r="A308" s="2" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C308" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="32">
       <c r="A309" s="2" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B309" s="13" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C309" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="144">
       <c r="A310" s="2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C310" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="144">
       <c r="A311" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C311" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="176">
       <c r="A312" s="2" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C312" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="64">
       <c r="A313" s="2" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C313" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="314" spans="1:3" ht="80">
       <c r="A314" s="2" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C314" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="315" spans="1:3" ht="64">
       <c r="A315" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C315" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="316" spans="1:3" ht="32">
       <c r="A316" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C316" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="16">
       <c r="A317" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B317" s="59" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="176">
       <c r="A318" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C318" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="208">
       <c r="A319" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C319" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="112">
       <c r="A320" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C320" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="365">
       <c r="A321" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C321" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="272">
       <c r="A322" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C322" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="96">
       <c r="A323" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C323" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="176">
       <c r="A324" s="2" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C324" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="32">
       <c r="A325" s="2" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C325" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
     </row>
     <row r="326" spans="1:3" ht="48">
       <c r="A326" s="2" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C326" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="176">
       <c r="A327" s="2" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C327" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="112">
       <c r="A328" s="2" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C328" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="329" spans="1:3" ht="80">
       <c r="A329" s="2" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C329" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="330" spans="1:3" ht="176">
       <c r="A330" s="2" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C330" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="331" spans="1:3" ht="32">
       <c r="A331" s="2" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C331" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="332" spans="1:3" ht="64">
       <c r="A332" s="2" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B332" s="13" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C332" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
     </row>
     <row r="333" spans="1:3" ht="160">
       <c r="A333" s="2" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B333" s="13" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C333" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="224">
       <c r="A334" s="2" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="C334" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>